<commit_message>
username was not being created
</commit_message>
<xml_diff>
--- a/documents/templates/bulk-upload/03-BulkUploadUser.xlsx
+++ b/documents/templates/bulk-upload/03-BulkUploadUser.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineshgajjar/Documents/Work/GitLab/YHWorks/Briot/clients/TMML/server/documents/templates/bulk-upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5752B931-236C-994C-AAFC-A9DFBF11DAB1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ADEB11-8635-E248-94B6-F9BF337D3790}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="1960" windowWidth="26840" windowHeight="15540" xr2:uid="{3B9B6560-6B0A-7549-BEDB-B7FFEA0F7BFE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Password</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>tmml</t>
+  </si>
+  <si>
+    <t>admin</t>
   </si>
 </sst>
 </file>
@@ -403,7 +406,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -428,7 +431,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
employee and user details added
</commit_message>
<xml_diff>
--- a/documents/templates/bulk-upload/03-BulkUploadUser.xlsx
+++ b/documents/templates/bulk-upload/03-BulkUploadUser.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineshgajjar/Documents/Work/GitLab/YHWorks/Briot/clients/TMML/server/documents/templates/bulk-upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ADEB11-8635-E248-94B6-F9BF337D3790}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2745AC-AA6A-044B-BC33-26371CFEFDB1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="1960" windowWidth="26840" windowHeight="15540" xr2:uid="{3B9B6560-6B0A-7549-BEDB-B7FFEA0F7BFE}"/>
+    <workbookView xWindow="4920" yWindow="1960" windowWidth="23500" windowHeight="15540" xr2:uid="{3B9B6560-6B0A-7549-BEDB-B7FFEA0F7BFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="39">
   <si>
     <t>Password</t>
   </si>
@@ -52,16 +52,126 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>Factory Maintenance</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>Machine Shop (Production)</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>Girisha C N</t>
+  </si>
+  <si>
+    <t>Srinivasachari.K</t>
+  </si>
+  <si>
+    <t>Bhoopathy .M</t>
+  </si>
+  <si>
+    <t>Shidlingaswami H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KIRAN V K </t>
+  </si>
+  <si>
+    <t>UMESH GAYAKWAD</t>
+  </si>
+  <si>
+    <t>santosh.angadaki</t>
+  </si>
+  <si>
+    <t>NAVEEN B</t>
+  </si>
+  <si>
+    <t>Veeresh Kurli</t>
+  </si>
+  <si>
+    <t>Siddalingesh M</t>
+  </si>
+  <si>
+    <t>MANJUNATH BP</t>
+  </si>
+  <si>
+    <t>Mahaveer Kadatti</t>
+  </si>
+  <si>
+    <t>Mahaveer Gali</t>
+  </si>
+  <si>
+    <t>SAYED SAIF ALI P</t>
+  </si>
+  <si>
+    <t>DUNDAYYA V HIREMATH</t>
+  </si>
+  <si>
+    <t>SHIVANAND NOORJEPPANAVAR</t>
+  </si>
+  <si>
+    <t>Santosh Arishinakar</t>
+  </si>
+  <si>
+    <t>PRAVEEN DATAR</t>
+  </si>
+  <si>
+    <t>SANTOSH JOGLEKAR</t>
+  </si>
+  <si>
+    <t>SANTOSH HATTI</t>
+  </si>
+  <si>
+    <t>SHRIKANT R</t>
+  </si>
+  <si>
+    <t>CHANDRU DANAPPANAVAR</t>
+  </si>
+  <si>
+    <t>VISHWANATH HIREMATH</t>
+  </si>
+  <si>
+    <t>BHARAMGOUDA ABALUR</t>
+  </si>
+  <si>
+    <t>SHRIDHAR CHANDARKAY</t>
+  </si>
+  <si>
+    <t>NAVEENKUMAR MS</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>Production</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,7 +185,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -83,14 +193,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -403,20 +552,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA153E1-58EC-D144-84B5-D3F67DA6696D}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
@@ -429,8 +582,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
@@ -441,6 +594,552 @@
       </c>
       <c r="D2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>730809</v>
+      </c>
+      <c r="B3" s="7" t="str">
+        <f>_xlfn.TEXTJOIN(,,A3, "@tmml", 2019)</f>
+        <v>730809@tmml2019</v>
+      </c>
+      <c r="C3" s="1">
+        <v>730809</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>731018</v>
+      </c>
+      <c r="B4" s="7" t="str">
+        <f t="shared" ref="B4:B28" si="0">_xlfn.TEXTJOIN(,,A4, "@tmml", 2019)</f>
+        <v>731018@tmml2019</v>
+      </c>
+      <c r="C4" s="1">
+        <v>731018</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>730869</v>
+      </c>
+      <c r="B5" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>730869@tmml2019</v>
+      </c>
+      <c r="C5" s="1">
+        <v>730869</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>731653</v>
+      </c>
+      <c r="B6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>731653@tmml2019</v>
+      </c>
+      <c r="C6" s="1">
+        <v>731653</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>731855</v>
+      </c>
+      <c r="B7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>731855@tmml2019</v>
+      </c>
+      <c r="C7" s="1">
+        <v>731855</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>732210</v>
+      </c>
+      <c r="B8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>732210@tmml2019</v>
+      </c>
+      <c r="C8" s="1">
+        <v>732210</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>732091</v>
+      </c>
+      <c r="B9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>732091@tmml2019</v>
+      </c>
+      <c r="C9" s="1">
+        <v>732091</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>731728</v>
+      </c>
+      <c r="B10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>731728@tmml2019</v>
+      </c>
+      <c r="C10" s="1">
+        <v>731728</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>731872</v>
+      </c>
+      <c r="B11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>731872@tmml2019</v>
+      </c>
+      <c r="C11" s="1">
+        <v>731872</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>731948</v>
+      </c>
+      <c r="B12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>731948@tmml2019</v>
+      </c>
+      <c r="C12" s="1">
+        <v>731948</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>730225</v>
+      </c>
+      <c r="B13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>730225@tmml2019</v>
+      </c>
+      <c r="C13" s="1">
+        <v>730225</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>730688</v>
+      </c>
+      <c r="B14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>730688@tmml2019</v>
+      </c>
+      <c r="C14" s="2">
+        <v>730688</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
+        <v>731131</v>
+      </c>
+      <c r="B15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>731131@tmml2019</v>
+      </c>
+      <c r="C15" s="2">
+        <v>731131</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>779392</v>
+      </c>
+      <c r="B16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>779392@tmml2019</v>
+      </c>
+      <c r="C16" s="1">
+        <v>779392</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>779395</v>
+      </c>
+      <c r="B17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>779395@tmml2019</v>
+      </c>
+      <c r="C17" s="1">
+        <v>779395</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>779414</v>
+      </c>
+      <c r="B18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>779414@tmml2019</v>
+      </c>
+      <c r="C18" s="1">
+        <v>779414</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>730101</v>
+      </c>
+      <c r="B19" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>730101@tmml2019</v>
+      </c>
+      <c r="C19" s="1">
+        <v>730101</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>730081</v>
+      </c>
+      <c r="B20" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>730081@tmml2019</v>
+      </c>
+      <c r="C20" s="1">
+        <v>730081</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>730124</v>
+      </c>
+      <c r="B21" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>730124@tmml2019</v>
+      </c>
+      <c r="C21" s="1">
+        <v>730124</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
+        <v>731450</v>
+      </c>
+      <c r="B22" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>731450@tmml2019</v>
+      </c>
+      <c r="C22" s="1">
+        <v>731450</v>
+      </c>
+      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
+        <v>731623</v>
+      </c>
+      <c r="B23" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>731623@tmml2019</v>
+      </c>
+      <c r="C23" s="1">
+        <v>731623</v>
+      </c>
+      <c r="D23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>730057</v>
+      </c>
+      <c r="B24" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>730057@tmml2019</v>
+      </c>
+      <c r="C24" s="1">
+        <v>730057</v>
+      </c>
+      <c r="D24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
+        <v>730113</v>
+      </c>
+      <c r="B25" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>730113@tmml2019</v>
+      </c>
+      <c r="C25" s="1">
+        <v>730113</v>
+      </c>
+      <c r="D25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
+        <v>730031</v>
+      </c>
+      <c r="B26" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>730031@tmml2019</v>
+      </c>
+      <c r="C26" s="1">
+        <v>730031</v>
+      </c>
+      <c r="D26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
+        <v>732184</v>
+      </c>
+      <c r="B27" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>732184@tmml2019</v>
+      </c>
+      <c r="C27" s="1">
+        <v>732184</v>
+      </c>
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>732253</v>
+      </c>
+      <c r="B28" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>732253@tmml2019</v>
+      </c>
+      <c r="C28" s="1">
+        <v>732253</v>
+      </c>
+      <c r="D28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>